<commit_message>
update registration form to make vaccine multiselect and update icons
</commit_message>
<xml_diff>
--- a/forms/app/covid_vaccine_registration.xlsx
+++ b/forms/app/covid_vaccine_registration.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="281">
   <si>
     <t>type</t>
   </si>
@@ -265,7 +265,7 @@
     <t>Have you received COVID-19 vaccine?</t>
   </si>
   <si>
-    <t>select_one vaccine_types</t>
+    <t>select_multiple vaccine_types</t>
   </si>
   <si>
     <t>covid_vaccine_type</t>
@@ -606,6 +606,12 @@
 selected(../non_vaccination_reason, 'breast_feeding') or 
 selected(../non_vaccination_reason, 'not_effective') or 
 selected(../non_vaccination_reason, 'other')</t>
+  </si>
+  <si>
+    <t>next_follow_up2</t>
+  </si>
+  <si>
+    <t>selected(../get_vaccine2, 'yes')</t>
   </si>
   <si>
     <t>n_vaccine_reach_out</t>
@@ -4617,52 +4623,64 @@
       <c r="AA82" s="20"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B83" s="15" t="s">
+      <c r="A83" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B83" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="C83" s="22" t="s">
+      <c r="C83" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="D83" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E83" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="D83" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E83" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="F83" s="7"/>
-      <c r="G83" s="7"/>
-      <c r="H83" s="7"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="7"/>
-      <c r="K83" s="7"/>
-      <c r="L83" s="7"/>
-      <c r="M83" s="7"/>
-      <c r="N83" s="7"/>
-      <c r="O83" s="7"/>
-      <c r="P83" s="7"/>
-      <c r="Q83" s="7"/>
-      <c r="R83" s="7"/>
-      <c r="S83" s="7"/>
-      <c r="T83" s="7"/>
-      <c r="U83" s="7"/>
-      <c r="V83" s="7"/>
-      <c r="W83" s="7"/>
-      <c r="X83" s="7"/>
-      <c r="Y83" s="7"/>
-      <c r="Z83" s="7"/>
-      <c r="AA83" s="7"/>
+      <c r="F83" s="28"/>
+      <c r="G83" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="H83" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="I83" s="20"/>
+      <c r="J83" s="28"/>
+      <c r="K83" s="28"/>
+      <c r="L83" s="28"/>
+      <c r="M83" s="28"/>
+      <c r="N83" s="28"/>
+      <c r="O83" s="28"/>
+      <c r="P83" s="28"/>
+      <c r="Q83" s="28"/>
+      <c r="R83" s="28"/>
+      <c r="S83" s="28"/>
+      <c r="T83" s="28"/>
+      <c r="U83" s="28"/>
+      <c r="V83" s="28"/>
+      <c r="W83" s="28"/>
+      <c r="X83" s="28"/>
+      <c r="Y83" s="28"/>
+      <c r="Z83" s="28"/>
+      <c r="AA83" s="28"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B84" s="13"/>
-      <c r="C84" s="14"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E84" s="18" t="s">
+        <v>199</v>
+      </c>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
@@ -4687,92 +4705,88 @@
       <c r="AA84" s="7"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B85" s="13"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="7"/>
+      <c r="K85" s="7"/>
+      <c r="L85" s="7"/>
+      <c r="M85" s="7"/>
+      <c r="N85" s="7"/>
+      <c r="O85" s="7"/>
+      <c r="P85" s="7"/>
+      <c r="Q85" s="7"/>
+      <c r="R85" s="7"/>
+      <c r="S85" s="7"/>
+      <c r="T85" s="7"/>
+      <c r="U85" s="7"/>
+      <c r="V85" s="7"/>
+      <c r="W85" s="7"/>
+      <c r="X85" s="7"/>
+      <c r="Y85" s="7"/>
+      <c r="Z85" s="7"/>
+      <c r="AA85" s="7"/>
+    </row>
+    <row r="86" ht="15.75" customHeight="1">
+      <c r="A86" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B85" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="3" t="s">
+      <c r="B86" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="G85" s="4"/>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="4"/>
-      <c r="K85" s="4"/>
-      <c r="L85" s="4"/>
-      <c r="M85" s="4"/>
-      <c r="N85" s="4"/>
-      <c r="O85" s="4"/>
-      <c r="P85" s="4"/>
-      <c r="Q85" s="4"/>
-      <c r="R85" s="4"/>
-      <c r="S85" s="4"/>
-      <c r="T85" s="4"/>
-      <c r="U85" s="4"/>
-      <c r="V85" s="4"/>
-      <c r="W85" s="4"/>
-      <c r="X85" s="4"/>
-      <c r="Y85" s="4"/>
-      <c r="Z85" s="4"/>
-      <c r="AA85" s="4"/>
-    </row>
-    <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C86" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
-      <c r="F86" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="G86" s="8"/>
-      <c r="H86" s="8"/>
-      <c r="I86" s="8"/>
-      <c r="J86" s="8"/>
-      <c r="K86" s="8"/>
-      <c r="L86" s="8"/>
-      <c r="M86" s="8"/>
-      <c r="N86" s="8"/>
-      <c r="O86" s="8"/>
-      <c r="P86" s="8"/>
-      <c r="Q86" s="8"/>
-      <c r="R86" s="8"/>
-      <c r="S86" s="8"/>
-      <c r="T86" s="8"/>
-      <c r="U86" s="8"/>
-      <c r="V86" s="8"/>
-      <c r="W86" s="8"/>
-      <c r="X86" s="8"/>
-      <c r="Y86" s="8"/>
-      <c r="Z86" s="8"/>
-      <c r="AA86" s="8"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="4"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="4"/>
+      <c r="Q86" s="4"/>
+      <c r="R86" s="4"/>
+      <c r="S86" s="4"/>
+      <c r="T86" s="4"/>
+      <c r="U86" s="4"/>
+      <c r="V86" s="4"/>
+      <c r="W86" s="4"/>
+      <c r="X86" s="4"/>
+      <c r="Y86" s="4"/>
+      <c r="Z86" s="4"/>
+      <c r="AA86" s="4"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="17" t="s">
         <v>71</v>
       </c>
       <c r="B87" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C87" s="21" t="s">
         <v>203</v>
-      </c>
-      <c r="C87" s="21" t="s">
-        <v>204</v>
       </c>
       <c r="D87" s="8"/>
       <c r="E87" s="8"/>
-      <c r="F87" s="8"/>
+      <c r="F87" s="29" t="s">
+        <v>204</v>
+      </c>
       <c r="G87" s="8"/>
       <c r="H87" s="8"/>
       <c r="I87" s="8"/>
@@ -4802,14 +4816,12 @@
       <c r="B88" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C88" s="21" t="s">
         <v>206</v>
       </c>
       <c r="D88" s="8"/>
       <c r="E88" s="8"/>
-      <c r="F88" s="7" t="s">
-        <v>207</v>
-      </c>
+      <c r="F88" s="8"/>
       <c r="G88" s="8"/>
       <c r="H88" s="8"/>
       <c r="I88" s="8"/>
@@ -4837,14 +4849,16 @@
         <v>71</v>
       </c>
       <c r="B89" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C89" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="D89" s="8"/>
       <c r="E89" s="8"/>
-      <c r="F89" s="8"/>
+      <c r="F89" s="7" t="s">
+        <v>209</v>
+      </c>
       <c r="G89" s="8"/>
       <c r="H89" s="8"/>
       <c r="I89" s="8"/>
@@ -4871,17 +4885,15 @@
       <c r="A90" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B90" s="21" t="s">
+      <c r="B90" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="C90" s="21" t="s">
-        <v>88</v>
+      <c r="C90" s="7" t="s">
+        <v>211</v>
       </c>
       <c r="D90" s="8"/>
       <c r="E90" s="8"/>
-      <c r="F90" s="21" t="s">
-        <v>211</v>
-      </c>
+      <c r="F90" s="8"/>
       <c r="G90" s="8"/>
       <c r="H90" s="8"/>
       <c r="I90" s="8"/>
@@ -4912,13 +4924,13 @@
         <v>212</v>
       </c>
       <c r="C91" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D91" s="8"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="D91" s="8"/>
-      <c r="E91" s="29" t="s">
-        <v>214</v>
-      </c>
-      <c r="F91" s="21"/>
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
       <c r="I91" s="8"/>
@@ -4946,14 +4958,14 @@
         <v>71</v>
       </c>
       <c r="B92" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="C92" s="21" t="s">
         <v>215</v>
-      </c>
-      <c r="C92" s="21" t="s">
-        <v>216</v>
       </c>
       <c r="D92" s="8"/>
       <c r="E92" s="29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F92" s="21"/>
       <c r="G92" s="8"/>
@@ -4983,14 +4995,14 @@
         <v>71</v>
       </c>
       <c r="B93" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="C93" s="21" t="s">
         <v>218</v>
-      </c>
-      <c r="C93" s="21" t="s">
-        <v>219</v>
       </c>
       <c r="D93" s="8"/>
       <c r="E93" s="29" t="s">
-        <v>123</v>
+        <v>219</v>
       </c>
       <c r="F93" s="21"/>
       <c r="G93" s="8"/>
@@ -5027,11 +5039,9 @@
       </c>
       <c r="D94" s="8"/>
       <c r="E94" s="29" t="s">
-        <v>222</v>
-      </c>
-      <c r="F94" s="21" t="s">
-        <v>211</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="F94" s="21"/>
       <c r="G94" s="8"/>
       <c r="H94" s="8"/>
       <c r="I94" s="8"/>
@@ -5059,16 +5069,18 @@
         <v>71</v>
       </c>
       <c r="B95" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C95" s="21" t="s">
         <v>223</v>
-      </c>
-      <c r="C95" s="21" t="s">
-        <v>224</v>
       </c>
       <c r="D95" s="8"/>
       <c r="E95" s="29" t="s">
-        <v>222</v>
-      </c>
-      <c r="F95" s="21"/>
+        <v>224</v>
+      </c>
+      <c r="F95" s="21" t="s">
+        <v>213</v>
+      </c>
       <c r="G95" s="8"/>
       <c r="H95" s="8"/>
       <c r="I95" s="8"/>
@@ -5092,64 +5104,72 @@
       <c r="AA95" s="8"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="11" t="s">
+      <c r="A96" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B96" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="C96" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="D96" s="8"/>
+      <c r="E96" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="F96" s="21"/>
+      <c r="G96" s="8"/>
+      <c r="H96" s="8"/>
+      <c r="I96" s="8"/>
+      <c r="J96" s="8"/>
+      <c r="K96" s="8"/>
+      <c r="L96" s="8"/>
+      <c r="M96" s="8"/>
+      <c r="N96" s="8"/>
+      <c r="O96" s="8"/>
+      <c r="P96" s="8"/>
+      <c r="Q96" s="8"/>
+      <c r="R96" s="8"/>
+      <c r="S96" s="8"/>
+      <c r="T96" s="8"/>
+      <c r="U96" s="8"/>
+      <c r="V96" s="8"/>
+      <c r="W96" s="8"/>
+      <c r="X96" s="8"/>
+      <c r="Y96" s="8"/>
+      <c r="Z96" s="8"/>
+      <c r="AA96" s="8"/>
+    </row>
+    <row r="97" ht="15.75" customHeight="1">
+      <c r="A97" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="4"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="4"/>
-      <c r="G96" s="4"/>
-      <c r="H96" s="4"/>
-      <c r="I96" s="4"/>
-      <c r="J96" s="4"/>
-      <c r="K96" s="4"/>
-      <c r="L96" s="4"/>
-      <c r="M96" s="4"/>
-      <c r="N96" s="4"/>
-      <c r="O96" s="4"/>
-      <c r="P96" s="4"/>
-      <c r="Q96" s="4"/>
-      <c r="R96" s="4"/>
-      <c r="S96" s="4"/>
-      <c r="T96" s="4"/>
-      <c r="U96" s="4"/>
-      <c r="V96" s="4"/>
-      <c r="W96" s="4"/>
-      <c r="X96" s="4"/>
-      <c r="Y96" s="4"/>
-      <c r="Z96" s="4"/>
-      <c r="AA96" s="4"/>
-    </row>
-    <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="30"/>
-      <c r="B97" s="30"/>
-      <c r="C97" s="30"/>
-      <c r="D97" s="30"/>
-      <c r="E97" s="30"/>
-      <c r="F97" s="30"/>
-      <c r="G97" s="30"/>
-      <c r="H97" s="30"/>
-      <c r="I97" s="30"/>
-      <c r="J97" s="30"/>
-      <c r="K97" s="30"/>
-      <c r="L97" s="30"/>
-      <c r="M97" s="30"/>
-      <c r="N97" s="30"/>
-      <c r="O97" s="30"/>
-      <c r="P97" s="30"/>
-      <c r="Q97" s="30"/>
-      <c r="R97" s="30"/>
-      <c r="S97" s="30"/>
-      <c r="T97" s="30"/>
-      <c r="U97" s="30"/>
-      <c r="V97" s="30"/>
-      <c r="W97" s="30"/>
-      <c r="X97" s="30"/>
-      <c r="Y97" s="30"/>
-      <c r="Z97" s="30"/>
-      <c r="AA97" s="30"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="4"/>
+      <c r="L97" s="4"/>
+      <c r="M97" s="4"/>
+      <c r="N97" s="4"/>
+      <c r="O97" s="4"/>
+      <c r="P97" s="4"/>
+      <c r="Q97" s="4"/>
+      <c r="R97" s="4"/>
+      <c r="S97" s="4"/>
+      <c r="T97" s="4"/>
+      <c r="U97" s="4"/>
+      <c r="V97" s="4"/>
+      <c r="W97" s="4"/>
+      <c r="X97" s="4"/>
+      <c r="Y97" s="4"/>
+      <c r="Z97" s="4"/>
+      <c r="AA97" s="4"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="30"/>
@@ -5386,7 +5406,7 @@
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="30"/>
       <c r="B106" s="30"/>
-      <c r="C106" s="14"/>
+      <c r="C106" s="30"/>
       <c r="D106" s="30"/>
       <c r="E106" s="30"/>
       <c r="F106" s="30"/>
@@ -5415,7 +5435,7 @@
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="30"/>
       <c r="B107" s="30"/>
-      <c r="C107" s="30"/>
+      <c r="C107" s="14"/>
       <c r="D107" s="30"/>
       <c r="E107" s="30"/>
       <c r="F107" s="30"/>
@@ -5678,7 +5698,7 @@
       <c r="B116" s="30"/>
       <c r="C116" s="30"/>
       <c r="D116" s="30"/>
-      <c r="E116" s="13"/>
+      <c r="E116" s="30"/>
       <c r="F116" s="30"/>
       <c r="G116" s="30"/>
       <c r="H116" s="30"/>
@@ -5707,7 +5727,7 @@
       <c r="B117" s="30"/>
       <c r="C117" s="30"/>
       <c r="D117" s="30"/>
-      <c r="E117" s="30"/>
+      <c r="E117" s="13"/>
       <c r="F117" s="30"/>
       <c r="G117" s="30"/>
       <c r="H117" s="30"/>
@@ -6113,7 +6133,7 @@
       <c r="B131" s="30"/>
       <c r="C131" s="30"/>
       <c r="D131" s="30"/>
-      <c r="E131" s="13"/>
+      <c r="E131" s="30"/>
       <c r="F131" s="30"/>
       <c r="G131" s="30"/>
       <c r="H131" s="30"/>
@@ -6200,7 +6220,7 @@
       <c r="B134" s="30"/>
       <c r="C134" s="30"/>
       <c r="D134" s="30"/>
-      <c r="E134" s="30"/>
+      <c r="E134" s="13"/>
       <c r="F134" s="30"/>
       <c r="G134" s="30"/>
       <c r="H134" s="30"/>
@@ -6544,62 +6564,62 @@
       <c r="AA145" s="30"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="7"/>
-      <c r="B146" s="7"/>
-      <c r="C146" s="7"/>
-      <c r="D146" s="31"/>
-      <c r="E146" s="31"/>
-      <c r="F146" s="31"/>
-      <c r="G146" s="31"/>
-      <c r="H146" s="31"/>
-      <c r="I146" s="31"/>
-      <c r="J146" s="31"/>
-      <c r="K146" s="31"/>
-      <c r="L146" s="31"/>
-      <c r="M146" s="31"/>
-      <c r="N146" s="31"/>
-      <c r="O146" s="31"/>
-      <c r="P146" s="31"/>
-      <c r="Q146" s="31"/>
-      <c r="R146" s="31"/>
-      <c r="S146" s="31"/>
-      <c r="T146" s="31"/>
-      <c r="U146" s="31"/>
-      <c r="V146" s="31"/>
-      <c r="W146" s="31"/>
-      <c r="X146" s="31"/>
-      <c r="Y146" s="31"/>
-      <c r="Z146" s="31"/>
-      <c r="AA146" s="31"/>
+      <c r="A146" s="30"/>
+      <c r="B146" s="30"/>
+      <c r="C146" s="30"/>
+      <c r="D146" s="30"/>
+      <c r="E146" s="30"/>
+      <c r="F146" s="30"/>
+      <c r="G146" s="30"/>
+      <c r="H146" s="30"/>
+      <c r="I146" s="30"/>
+      <c r="J146" s="30"/>
+      <c r="K146" s="30"/>
+      <c r="L146" s="30"/>
+      <c r="M146" s="30"/>
+      <c r="N146" s="30"/>
+      <c r="O146" s="30"/>
+      <c r="P146" s="30"/>
+      <c r="Q146" s="30"/>
+      <c r="R146" s="30"/>
+      <c r="S146" s="30"/>
+      <c r="T146" s="30"/>
+      <c r="U146" s="30"/>
+      <c r="V146" s="30"/>
+      <c r="W146" s="30"/>
+      <c r="X146" s="30"/>
+      <c r="Y146" s="30"/>
+      <c r="Z146" s="30"/>
+      <c r="AA146" s="30"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="30"/>
-      <c r="B147" s="30"/>
+      <c r="A147" s="7"/>
+      <c r="B147" s="7"/>
       <c r="C147" s="7"/>
-      <c r="D147" s="30"/>
-      <c r="E147" s="30"/>
-      <c r="F147" s="30"/>
-      <c r="G147" s="30"/>
-      <c r="H147" s="30"/>
-      <c r="I147" s="30"/>
-      <c r="J147" s="30"/>
-      <c r="K147" s="30"/>
-      <c r="L147" s="30"/>
-      <c r="M147" s="30"/>
-      <c r="N147" s="30"/>
-      <c r="O147" s="30"/>
-      <c r="P147" s="30"/>
-      <c r="Q147" s="30"/>
-      <c r="R147" s="30"/>
-      <c r="S147" s="30"/>
-      <c r="T147" s="30"/>
-      <c r="U147" s="30"/>
-      <c r="V147" s="30"/>
-      <c r="W147" s="30"/>
-      <c r="X147" s="30"/>
-      <c r="Y147" s="30"/>
-      <c r="Z147" s="30"/>
-      <c r="AA147" s="30"/>
+      <c r="D147" s="31"/>
+      <c r="E147" s="31"/>
+      <c r="F147" s="31"/>
+      <c r="G147" s="31"/>
+      <c r="H147" s="31"/>
+      <c r="I147" s="31"/>
+      <c r="J147" s="31"/>
+      <c r="K147" s="31"/>
+      <c r="L147" s="31"/>
+      <c r="M147" s="31"/>
+      <c r="N147" s="31"/>
+      <c r="O147" s="31"/>
+      <c r="P147" s="31"/>
+      <c r="Q147" s="31"/>
+      <c r="R147" s="31"/>
+      <c r="S147" s="31"/>
+      <c r="T147" s="31"/>
+      <c r="U147" s="31"/>
+      <c r="V147" s="31"/>
+      <c r="W147" s="31"/>
+      <c r="X147" s="31"/>
+      <c r="Y147" s="31"/>
+      <c r="Z147" s="31"/>
+      <c r="AA147" s="31"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="30"/>
@@ -6718,9 +6738,9 @@
       <c r="AA151" s="30"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="7"/>
+      <c r="A152" s="30"/>
       <c r="B152" s="30"/>
-      <c r="C152" s="14"/>
+      <c r="C152" s="7"/>
       <c r="D152" s="30"/>
       <c r="E152" s="30"/>
       <c r="F152" s="30"/>
@@ -6747,9 +6767,9 @@
       <c r="AA152" s="30"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="30"/>
+      <c r="A153" s="7"/>
       <c r="B153" s="30"/>
-      <c r="C153" s="30"/>
+      <c r="C153" s="14"/>
       <c r="D153" s="30"/>
       <c r="E153" s="30"/>
       <c r="F153" s="30"/>
@@ -6776,33 +6796,33 @@
       <c r="AA153" s="30"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="7"/>
-      <c r="B154" s="7"/>
-      <c r="C154" s="7"/>
-      <c r="D154" s="7"/>
-      <c r="E154" s="7"/>
-      <c r="F154" s="7"/>
-      <c r="G154" s="7"/>
-      <c r="H154" s="7"/>
-      <c r="I154" s="7"/>
-      <c r="J154" s="7"/>
-      <c r="K154" s="7"/>
-      <c r="L154" s="7"/>
-      <c r="M154" s="7"/>
-      <c r="N154" s="7"/>
-      <c r="O154" s="7"/>
-      <c r="P154" s="7"/>
-      <c r="Q154" s="7"/>
-      <c r="R154" s="7"/>
-      <c r="S154" s="7"/>
-      <c r="T154" s="7"/>
-      <c r="U154" s="7"/>
-      <c r="V154" s="7"/>
-      <c r="W154" s="7"/>
-      <c r="X154" s="7"/>
-      <c r="Y154" s="7"/>
-      <c r="Z154" s="7"/>
-      <c r="AA154" s="7"/>
+      <c r="A154" s="30"/>
+      <c r="B154" s="30"/>
+      <c r="C154" s="30"/>
+      <c r="D154" s="30"/>
+      <c r="E154" s="30"/>
+      <c r="F154" s="30"/>
+      <c r="G154" s="30"/>
+      <c r="H154" s="30"/>
+      <c r="I154" s="30"/>
+      <c r="J154" s="30"/>
+      <c r="K154" s="30"/>
+      <c r="L154" s="30"/>
+      <c r="M154" s="30"/>
+      <c r="N154" s="30"/>
+      <c r="O154" s="30"/>
+      <c r="P154" s="30"/>
+      <c r="Q154" s="30"/>
+      <c r="R154" s="30"/>
+      <c r="S154" s="30"/>
+      <c r="T154" s="30"/>
+      <c r="U154" s="30"/>
+      <c r="V154" s="30"/>
+      <c r="W154" s="30"/>
+      <c r="X154" s="30"/>
+      <c r="Y154" s="30"/>
+      <c r="Z154" s="30"/>
+      <c r="AA154" s="30"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="7"/>
@@ -6865,7 +6885,7 @@
     <row r="157" ht="15.75" customHeight="1">
       <c r="A157" s="7"/>
       <c r="B157" s="7"/>
-      <c r="C157" s="14"/>
+      <c r="C157" s="7"/>
       <c r="D157" s="7"/>
       <c r="E157" s="7"/>
       <c r="F157" s="7"/>
@@ -6894,7 +6914,7 @@
     <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="7"/>
       <c r="B158" s="7"/>
-      <c r="C158" s="7"/>
+      <c r="C158" s="14"/>
       <c r="D158" s="7"/>
       <c r="E158" s="7"/>
       <c r="F158" s="7"/>
@@ -6922,90 +6942,90 @@
     </row>
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="7"/>
-      <c r="B159" s="30"/>
-      <c r="C159" s="14"/>
-      <c r="D159" s="30"/>
-      <c r="E159" s="30"/>
-      <c r="F159" s="30"/>
-      <c r="G159" s="30"/>
-      <c r="H159" s="30"/>
-      <c r="I159" s="30"/>
-      <c r="J159" s="30"/>
-      <c r="K159" s="30"/>
-      <c r="L159" s="30"/>
-      <c r="M159" s="30"/>
-      <c r="N159" s="30"/>
-      <c r="O159" s="30"/>
-      <c r="P159" s="30"/>
-      <c r="Q159" s="30"/>
-      <c r="R159" s="30"/>
-      <c r="S159" s="30"/>
-      <c r="T159" s="30"/>
-      <c r="U159" s="30"/>
-      <c r="V159" s="30"/>
-      <c r="W159" s="30"/>
-      <c r="X159" s="30"/>
-      <c r="Y159" s="30"/>
-      <c r="Z159" s="30"/>
-      <c r="AA159" s="30"/>
+      <c r="B159" s="7"/>
+      <c r="C159" s="7"/>
+      <c r="D159" s="7"/>
+      <c r="E159" s="7"/>
+      <c r="F159" s="7"/>
+      <c r="G159" s="7"/>
+      <c r="H159" s="7"/>
+      <c r="I159" s="7"/>
+      <c r="J159" s="7"/>
+      <c r="K159" s="7"/>
+      <c r="L159" s="7"/>
+      <c r="M159" s="7"/>
+      <c r="N159" s="7"/>
+      <c r="O159" s="7"/>
+      <c r="P159" s="7"/>
+      <c r="Q159" s="7"/>
+      <c r="R159" s="7"/>
+      <c r="S159" s="7"/>
+      <c r="T159" s="7"/>
+      <c r="U159" s="7"/>
+      <c r="V159" s="7"/>
+      <c r="W159" s="7"/>
+      <c r="X159" s="7"/>
+      <c r="Y159" s="7"/>
+      <c r="Z159" s="7"/>
+      <c r="AA159" s="7"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="7"/>
-      <c r="B160" s="7"/>
-      <c r="C160" s="7"/>
-      <c r="D160" s="7"/>
-      <c r="E160" s="7"/>
-      <c r="F160" s="7"/>
-      <c r="G160" s="7"/>
-      <c r="H160" s="7"/>
-      <c r="I160" s="7"/>
-      <c r="J160" s="7"/>
-      <c r="K160" s="7"/>
-      <c r="L160" s="7"/>
-      <c r="M160" s="7"/>
-      <c r="N160" s="7"/>
-      <c r="O160" s="7"/>
-      <c r="P160" s="7"/>
-      <c r="Q160" s="7"/>
-      <c r="R160" s="7"/>
-      <c r="S160" s="7"/>
-      <c r="T160" s="7"/>
-      <c r="U160" s="7"/>
-      <c r="V160" s="7"/>
-      <c r="W160" s="7"/>
-      <c r="X160" s="7"/>
-      <c r="Y160" s="7"/>
-      <c r="Z160" s="7"/>
-      <c r="AA160" s="7"/>
+      <c r="B160" s="30"/>
+      <c r="C160" s="14"/>
+      <c r="D160" s="30"/>
+      <c r="E160" s="30"/>
+      <c r="F160" s="30"/>
+      <c r="G160" s="30"/>
+      <c r="H160" s="30"/>
+      <c r="I160" s="30"/>
+      <c r="J160" s="30"/>
+      <c r="K160" s="30"/>
+      <c r="L160" s="30"/>
+      <c r="M160" s="30"/>
+      <c r="N160" s="30"/>
+      <c r="O160" s="30"/>
+      <c r="P160" s="30"/>
+      <c r="Q160" s="30"/>
+      <c r="R160" s="30"/>
+      <c r="S160" s="30"/>
+      <c r="T160" s="30"/>
+      <c r="U160" s="30"/>
+      <c r="V160" s="30"/>
+      <c r="W160" s="30"/>
+      <c r="X160" s="30"/>
+      <c r="Y160" s="30"/>
+      <c r="Z160" s="30"/>
+      <c r="AA160" s="30"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="7"/>
-      <c r="B161" s="30"/>
-      <c r="C161" s="30"/>
-      <c r="D161" s="30"/>
-      <c r="E161" s="30"/>
-      <c r="F161" s="30"/>
-      <c r="G161" s="30"/>
-      <c r="H161" s="30"/>
-      <c r="I161" s="30"/>
-      <c r="J161" s="30"/>
-      <c r="K161" s="30"/>
-      <c r="L161" s="30"/>
-      <c r="M161" s="30"/>
-      <c r="N161" s="30"/>
-      <c r="O161" s="30"/>
-      <c r="P161" s="30"/>
-      <c r="Q161" s="30"/>
-      <c r="R161" s="30"/>
-      <c r="S161" s="30"/>
-      <c r="T161" s="30"/>
-      <c r="U161" s="30"/>
-      <c r="V161" s="30"/>
-      <c r="W161" s="30"/>
-      <c r="X161" s="30"/>
-      <c r="Y161" s="30"/>
-      <c r="Z161" s="30"/>
-      <c r="AA161" s="30"/>
+      <c r="B161" s="7"/>
+      <c r="C161" s="7"/>
+      <c r="D161" s="7"/>
+      <c r="E161" s="7"/>
+      <c r="F161" s="7"/>
+      <c r="G161" s="7"/>
+      <c r="H161" s="7"/>
+      <c r="I161" s="7"/>
+      <c r="J161" s="7"/>
+      <c r="K161" s="7"/>
+      <c r="L161" s="7"/>
+      <c r="M161" s="7"/>
+      <c r="N161" s="7"/>
+      <c r="O161" s="7"/>
+      <c r="P161" s="7"/>
+      <c r="Q161" s="7"/>
+      <c r="R161" s="7"/>
+      <c r="S161" s="7"/>
+      <c r="T161" s="7"/>
+      <c r="U161" s="7"/>
+      <c r="V161" s="7"/>
+      <c r="W161" s="7"/>
+      <c r="X161" s="7"/>
+      <c r="Y161" s="7"/>
+      <c r="Z161" s="7"/>
+      <c r="AA161" s="7"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="7"/>
@@ -7068,7 +7088,7 @@
     <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="7"/>
       <c r="B164" s="30"/>
-      <c r="C164" s="14"/>
+      <c r="C164" s="30"/>
       <c r="D164" s="30"/>
       <c r="E164" s="30"/>
       <c r="F164" s="30"/>
@@ -7097,7 +7117,7 @@
     <row r="165" ht="15.75" customHeight="1">
       <c r="A165" s="7"/>
       <c r="B165" s="30"/>
-      <c r="C165" s="30"/>
+      <c r="C165" s="14"/>
       <c r="D165" s="30"/>
       <c r="E165" s="30"/>
       <c r="F165" s="30"/>
@@ -7213,7 +7233,7 @@
     <row r="169" ht="15.75" customHeight="1">
       <c r="A169" s="7"/>
       <c r="B169" s="30"/>
-      <c r="C169" s="14"/>
+      <c r="C169" s="30"/>
       <c r="D169" s="30"/>
       <c r="E169" s="30"/>
       <c r="F169" s="30"/>
@@ -7242,7 +7262,7 @@
     <row r="170" ht="15.75" customHeight="1">
       <c r="A170" s="7"/>
       <c r="B170" s="30"/>
-      <c r="C170" s="30"/>
+      <c r="C170" s="14"/>
       <c r="D170" s="30"/>
       <c r="E170" s="30"/>
       <c r="F170" s="30"/>
@@ -7271,7 +7291,7 @@
     <row r="171" ht="15.75" customHeight="1">
       <c r="A171" s="7"/>
       <c r="B171" s="30"/>
-      <c r="C171" s="14"/>
+      <c r="C171" s="30"/>
       <c r="D171" s="30"/>
       <c r="E171" s="30"/>
       <c r="F171" s="30"/>
@@ -7300,7 +7320,7 @@
     <row r="172" ht="15.75" customHeight="1">
       <c r="A172" s="7"/>
       <c r="B172" s="30"/>
-      <c r="C172" s="30"/>
+      <c r="C172" s="14"/>
       <c r="D172" s="30"/>
       <c r="E172" s="30"/>
       <c r="F172" s="30"/>
@@ -7329,7 +7349,7 @@
     <row r="173" ht="15.75" customHeight="1">
       <c r="A173" s="7"/>
       <c r="B173" s="30"/>
-      <c r="C173" s="7"/>
+      <c r="C173" s="30"/>
       <c r="D173" s="30"/>
       <c r="E173" s="30"/>
       <c r="F173" s="30"/>
@@ -7357,32 +7377,32 @@
     </row>
     <row r="174" ht="15.75" customHeight="1">
       <c r="A174" s="7"/>
-      <c r="B174" s="7"/>
+      <c r="B174" s="30"/>
       <c r="C174" s="7"/>
-      <c r="D174" s="7"/>
-      <c r="E174" s="7"/>
-      <c r="F174" s="7"/>
-      <c r="G174" s="7"/>
-      <c r="H174" s="7"/>
-      <c r="I174" s="7"/>
-      <c r="J174" s="7"/>
-      <c r="K174" s="7"/>
-      <c r="L174" s="7"/>
-      <c r="M174" s="7"/>
-      <c r="N174" s="7"/>
-      <c r="O174" s="7"/>
-      <c r="P174" s="7"/>
-      <c r="Q174" s="7"/>
-      <c r="R174" s="7"/>
-      <c r="S174" s="7"/>
-      <c r="T174" s="7"/>
-      <c r="U174" s="7"/>
-      <c r="V174" s="7"/>
-      <c r="W174" s="7"/>
-      <c r="X174" s="7"/>
-      <c r="Y174" s="7"/>
-      <c r="Z174" s="7"/>
-      <c r="AA174" s="7"/>
+      <c r="D174" s="30"/>
+      <c r="E174" s="30"/>
+      <c r="F174" s="30"/>
+      <c r="G174" s="30"/>
+      <c r="H174" s="30"/>
+      <c r="I174" s="30"/>
+      <c r="J174" s="30"/>
+      <c r="K174" s="30"/>
+      <c r="L174" s="30"/>
+      <c r="M174" s="30"/>
+      <c r="N174" s="30"/>
+      <c r="O174" s="30"/>
+      <c r="P174" s="30"/>
+      <c r="Q174" s="30"/>
+      <c r="R174" s="30"/>
+      <c r="S174" s="30"/>
+      <c r="T174" s="30"/>
+      <c r="U174" s="30"/>
+      <c r="V174" s="30"/>
+      <c r="W174" s="30"/>
+      <c r="X174" s="30"/>
+      <c r="Y174" s="30"/>
+      <c r="Z174" s="30"/>
+      <c r="AA174" s="30"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
       <c r="A175" s="7"/>
@@ -7474,7 +7494,7 @@
     <row r="178" ht="15.75" customHeight="1">
       <c r="A178" s="7"/>
       <c r="B178" s="7"/>
-      <c r="C178" s="14"/>
+      <c r="C178" s="7"/>
       <c r="D178" s="7"/>
       <c r="E178" s="7"/>
       <c r="F178" s="7"/>
@@ -7561,7 +7581,7 @@
     <row r="181" ht="15.75" customHeight="1">
       <c r="A181" s="7"/>
       <c r="B181" s="7"/>
-      <c r="C181" s="7"/>
+      <c r="C181" s="14"/>
       <c r="D181" s="7"/>
       <c r="E181" s="7"/>
       <c r="F181" s="7"/>
@@ -7851,7 +7871,7 @@
     <row r="191" ht="15.75" customHeight="1">
       <c r="A191" s="7"/>
       <c r="B191" s="7"/>
-      <c r="C191" s="14"/>
+      <c r="C191" s="7"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
       <c r="F191" s="7"/>
@@ -7909,7 +7929,7 @@
     <row r="193" ht="15.75" customHeight="1">
       <c r="A193" s="7"/>
       <c r="B193" s="7"/>
-      <c r="C193" s="7"/>
+      <c r="C193" s="14"/>
       <c r="D193" s="7"/>
       <c r="E193" s="7"/>
       <c r="F193" s="7"/>
@@ -7996,7 +8016,7 @@
     <row r="196" ht="15.75" customHeight="1">
       <c r="A196" s="7"/>
       <c r="B196" s="7"/>
-      <c r="C196" s="13"/>
+      <c r="C196" s="7"/>
       <c r="D196" s="7"/>
       <c r="E196" s="7"/>
       <c r="F196" s="7"/>
@@ -8083,7 +8103,7 @@
     <row r="199" ht="15.75" customHeight="1">
       <c r="A199" s="7"/>
       <c r="B199" s="7"/>
-      <c r="C199" s="7"/>
+      <c r="C199" s="13"/>
       <c r="D199" s="7"/>
       <c r="E199" s="7"/>
       <c r="F199" s="7"/>
@@ -8112,7 +8132,7 @@
     <row r="200" ht="15.75" customHeight="1">
       <c r="A200" s="7"/>
       <c r="B200" s="7"/>
-      <c r="C200" s="13"/>
+      <c r="C200" s="7"/>
       <c r="D200" s="7"/>
       <c r="E200" s="7"/>
       <c r="F200" s="7"/>
@@ -8143,7 +8163,7 @@
       <c r="B201" s="7"/>
       <c r="C201" s="13"/>
       <c r="D201" s="7"/>
-      <c r="E201" s="13"/>
+      <c r="E201" s="7"/>
       <c r="F201" s="7"/>
       <c r="G201" s="7"/>
       <c r="H201" s="7"/>
@@ -8170,9 +8190,9 @@
     <row r="202" ht="15.75" customHeight="1">
       <c r="A202" s="7"/>
       <c r="B202" s="7"/>
-      <c r="C202" s="7"/>
+      <c r="C202" s="13"/>
       <c r="D202" s="7"/>
-      <c r="E202" s="7"/>
+      <c r="E202" s="13"/>
       <c r="F202" s="7"/>
       <c r="G202" s="7"/>
       <c r="H202" s="7"/>
@@ -8402,7 +8422,7 @@
     <row r="210" ht="15.75" customHeight="1">
       <c r="A210" s="7"/>
       <c r="B210" s="7"/>
-      <c r="C210" s="14"/>
+      <c r="C210" s="7"/>
       <c r="D210" s="7"/>
       <c r="E210" s="7"/>
       <c r="F210" s="7"/>
@@ -8431,7 +8451,7 @@
     <row r="211" ht="15.75" customHeight="1">
       <c r="A211" s="7"/>
       <c r="B211" s="7"/>
-      <c r="C211" s="7"/>
+      <c r="C211" s="14"/>
       <c r="D211" s="7"/>
       <c r="E211" s="7"/>
       <c r="F211" s="7"/>
@@ -8460,7 +8480,7 @@
     <row r="212" ht="15.75" customHeight="1">
       <c r="A212" s="7"/>
       <c r="B212" s="7"/>
-      <c r="C212" s="14"/>
+      <c r="C212" s="7"/>
       <c r="D212" s="7"/>
       <c r="E212" s="7"/>
       <c r="F212" s="7"/>
@@ -8489,7 +8509,7 @@
     <row r="213" ht="15.75" customHeight="1">
       <c r="A213" s="7"/>
       <c r="B213" s="7"/>
-      <c r="C213" s="13"/>
+      <c r="C213" s="14"/>
       <c r="D213" s="7"/>
       <c r="E213" s="7"/>
       <c r="F213" s="7"/>
@@ -8518,7 +8538,7 @@
     <row r="214" ht="15.75" customHeight="1">
       <c r="A214" s="7"/>
       <c r="B214" s="7"/>
-      <c r="C214" s="14"/>
+      <c r="C214" s="13"/>
       <c r="D214" s="7"/>
       <c r="E214" s="7"/>
       <c r="F214" s="7"/>
@@ -8547,7 +8567,7 @@
     <row r="215" ht="15.75" customHeight="1">
       <c r="A215" s="7"/>
       <c r="B215" s="7"/>
-      <c r="C215" s="13"/>
+      <c r="C215" s="14"/>
       <c r="D215" s="7"/>
       <c r="E215" s="7"/>
       <c r="F215" s="7"/>
@@ -8576,7 +8596,7 @@
     <row r="216" ht="15.75" customHeight="1">
       <c r="A216" s="7"/>
       <c r="B216" s="7"/>
-      <c r="C216" s="14"/>
+      <c r="C216" s="13"/>
       <c r="D216" s="7"/>
       <c r="E216" s="7"/>
       <c r="F216" s="7"/>
@@ -8605,7 +8625,7 @@
     <row r="217" ht="15.75" customHeight="1">
       <c r="A217" s="7"/>
       <c r="B217" s="7"/>
-      <c r="C217" s="7"/>
+      <c r="C217" s="14"/>
       <c r="D217" s="7"/>
       <c r="E217" s="7"/>
       <c r="F217" s="7"/>
@@ -8634,7 +8654,7 @@
     <row r="218" ht="15.75" customHeight="1">
       <c r="A218" s="7"/>
       <c r="B218" s="7"/>
-      <c r="C218" s="14"/>
+      <c r="C218" s="7"/>
       <c r="D218" s="7"/>
       <c r="E218" s="7"/>
       <c r="F218" s="7"/>
@@ -8663,7 +8683,7 @@
     <row r="219" ht="15.75" customHeight="1">
       <c r="A219" s="7"/>
       <c r="B219" s="7"/>
-      <c r="C219" s="7"/>
+      <c r="C219" s="14"/>
       <c r="D219" s="7"/>
       <c r="E219" s="7"/>
       <c r="F219" s="7"/>
@@ -8692,7 +8712,7 @@
     <row r="220" ht="15.75" customHeight="1">
       <c r="A220" s="7"/>
       <c r="B220" s="7"/>
-      <c r="C220" s="14"/>
+      <c r="C220" s="7"/>
       <c r="D220" s="7"/>
       <c r="E220" s="7"/>
       <c r="F220" s="7"/>
@@ -8719,67 +8739,67 @@
       <c r="AA220" s="7"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="32"/>
-      <c r="B221" s="32"/>
-      <c r="C221" s="32"/>
-      <c r="D221" s="32"/>
-      <c r="E221" s="32"/>
-      <c r="F221" s="32"/>
-      <c r="G221" s="32"/>
-      <c r="H221" s="32"/>
-      <c r="I221" s="32"/>
-      <c r="J221" s="32"/>
-      <c r="K221" s="32"/>
-      <c r="L221" s="32"/>
-      <c r="M221" s="32"/>
-      <c r="N221" s="32"/>
-      <c r="O221" s="32"/>
-      <c r="P221" s="32"/>
-      <c r="Q221" s="32"/>
-      <c r="R221" s="32"/>
-      <c r="S221" s="32"/>
-      <c r="T221" s="32"/>
-      <c r="U221" s="32"/>
-      <c r="V221" s="32"/>
-      <c r="W221" s="32"/>
-      <c r="X221" s="32"/>
-      <c r="Y221" s="32"/>
-      <c r="Z221" s="32"/>
-      <c r="AA221" s="32"/>
+      <c r="A221" s="7"/>
+      <c r="B221" s="7"/>
+      <c r="C221" s="14"/>
+      <c r="D221" s="7"/>
+      <c r="E221" s="7"/>
+      <c r="F221" s="7"/>
+      <c r="G221" s="7"/>
+      <c r="H221" s="7"/>
+      <c r="I221" s="7"/>
+      <c r="J221" s="7"/>
+      <c r="K221" s="7"/>
+      <c r="L221" s="7"/>
+      <c r="M221" s="7"/>
+      <c r="N221" s="7"/>
+      <c r="O221" s="7"/>
+      <c r="P221" s="7"/>
+      <c r="Q221" s="7"/>
+      <c r="R221" s="7"/>
+      <c r="S221" s="7"/>
+      <c r="T221" s="7"/>
+      <c r="U221" s="7"/>
+      <c r="V221" s="7"/>
+      <c r="W221" s="7"/>
+      <c r="X221" s="7"/>
+      <c r="Y221" s="7"/>
+      <c r="Z221" s="7"/>
+      <c r="AA221" s="7"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="7"/>
-      <c r="B222" s="7"/>
-      <c r="C222" s="7"/>
-      <c r="D222" s="7"/>
-      <c r="E222" s="7"/>
-      <c r="F222" s="7"/>
-      <c r="G222" s="7"/>
-      <c r="H222" s="7"/>
-      <c r="I222" s="7"/>
-      <c r="J222" s="7"/>
-      <c r="K222" s="7"/>
-      <c r="L222" s="7"/>
-      <c r="M222" s="7"/>
-      <c r="N222" s="7"/>
-      <c r="O222" s="7"/>
-      <c r="P222" s="7"/>
-      <c r="Q222" s="7"/>
-      <c r="R222" s="7"/>
-      <c r="S222" s="7"/>
-      <c r="T222" s="7"/>
-      <c r="U222" s="7"/>
-      <c r="V222" s="7"/>
-      <c r="W222" s="7"/>
-      <c r="X222" s="7"/>
-      <c r="Y222" s="7"/>
-      <c r="Z222" s="7"/>
-      <c r="AA222" s="7"/>
+      <c r="A222" s="32"/>
+      <c r="B222" s="32"/>
+      <c r="C222" s="32"/>
+      <c r="D222" s="32"/>
+      <c r="E222" s="32"/>
+      <c r="F222" s="32"/>
+      <c r="G222" s="32"/>
+      <c r="H222" s="32"/>
+      <c r="I222" s="32"/>
+      <c r="J222" s="32"/>
+      <c r="K222" s="32"/>
+      <c r="L222" s="32"/>
+      <c r="M222" s="32"/>
+      <c r="N222" s="32"/>
+      <c r="O222" s="32"/>
+      <c r="P222" s="32"/>
+      <c r="Q222" s="32"/>
+      <c r="R222" s="32"/>
+      <c r="S222" s="32"/>
+      <c r="T222" s="32"/>
+      <c r="U222" s="32"/>
+      <c r="V222" s="32"/>
+      <c r="W222" s="32"/>
+      <c r="X222" s="32"/>
+      <c r="Y222" s="32"/>
+      <c r="Z222" s="32"/>
+      <c r="AA222" s="32"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
       <c r="A223" s="7"/>
       <c r="B223" s="7"/>
-      <c r="C223" s="14"/>
+      <c r="C223" s="7"/>
       <c r="D223" s="7"/>
       <c r="E223" s="7"/>
       <c r="F223" s="7"/>
@@ -8808,7 +8828,7 @@
     <row r="224" ht="15.75" customHeight="1">
       <c r="A224" s="7"/>
       <c r="B224" s="7"/>
-      <c r="C224" s="7"/>
+      <c r="C224" s="14"/>
       <c r="D224" s="7"/>
       <c r="E224" s="7"/>
       <c r="F224" s="7"/>
@@ -8837,7 +8857,7 @@
     <row r="225" ht="15.75" customHeight="1">
       <c r="A225" s="7"/>
       <c r="B225" s="7"/>
-      <c r="C225" s="14"/>
+      <c r="C225" s="7"/>
       <c r="D225" s="7"/>
       <c r="E225" s="7"/>
       <c r="F225" s="7"/>
@@ -8866,7 +8886,7 @@
     <row r="226" ht="15.75" customHeight="1">
       <c r="A226" s="7"/>
       <c r="B226" s="7"/>
-      <c r="C226" s="13"/>
+      <c r="C226" s="14"/>
       <c r="D226" s="7"/>
       <c r="E226" s="7"/>
       <c r="F226" s="7"/>
@@ -8895,7 +8915,7 @@
     <row r="227" ht="15.75" customHeight="1">
       <c r="A227" s="7"/>
       <c r="B227" s="7"/>
-      <c r="C227" s="14"/>
+      <c r="C227" s="13"/>
       <c r="D227" s="7"/>
       <c r="E227" s="7"/>
       <c r="F227" s="7"/>
@@ -8924,38 +8944,38 @@
     <row r="228" ht="15.75" customHeight="1">
       <c r="A228" s="7"/>
       <c r="B228" s="7"/>
-      <c r="C228" s="7"/>
-      <c r="D228" s="31"/>
+      <c r="C228" s="14"/>
+      <c r="D228" s="7"/>
       <c r="E228" s="7"/>
-      <c r="F228" s="31"/>
-      <c r="G228" s="31"/>
-      <c r="H228" s="31"/>
+      <c r="F228" s="7"/>
+      <c r="G228" s="7"/>
+      <c r="H228" s="7"/>
       <c r="I228" s="7"/>
-      <c r="J228" s="31"/>
-      <c r="K228" s="31"/>
-      <c r="L228" s="31"/>
-      <c r="M228" s="31"/>
-      <c r="N228" s="31"/>
-      <c r="O228" s="31"/>
-      <c r="P228" s="31"/>
-      <c r="Q228" s="31"/>
-      <c r="R228" s="31"/>
-      <c r="S228" s="31"/>
-      <c r="T228" s="31"/>
-      <c r="U228" s="31"/>
-      <c r="V228" s="31"/>
-      <c r="W228" s="31"/>
-      <c r="X228" s="31"/>
-      <c r="Y228" s="31"/>
-      <c r="Z228" s="31"/>
-      <c r="AA228" s="31"/>
+      <c r="J228" s="7"/>
+      <c r="K228" s="7"/>
+      <c r="L228" s="7"/>
+      <c r="M228" s="7"/>
+      <c r="N228" s="7"/>
+      <c r="O228" s="7"/>
+      <c r="P228" s="7"/>
+      <c r="Q228" s="7"/>
+      <c r="R228" s="7"/>
+      <c r="S228" s="7"/>
+      <c r="T228" s="7"/>
+      <c r="U228" s="7"/>
+      <c r="V228" s="7"/>
+      <c r="W228" s="7"/>
+      <c r="X228" s="7"/>
+      <c r="Y228" s="7"/>
+      <c r="Z228" s="7"/>
+      <c r="AA228" s="7"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
       <c r="A229" s="7"/>
       <c r="B229" s="7"/>
-      <c r="C229" s="14"/>
+      <c r="C229" s="7"/>
       <c r="D229" s="31"/>
-      <c r="E229" s="31"/>
+      <c r="E229" s="7"/>
       <c r="F229" s="31"/>
       <c r="G229" s="31"/>
       <c r="H229" s="31"/>
@@ -8982,13 +9002,13 @@
     <row r="230" ht="15.75" customHeight="1">
       <c r="A230" s="7"/>
       <c r="B230" s="7"/>
-      <c r="C230" s="7"/>
+      <c r="C230" s="14"/>
       <c r="D230" s="31"/>
-      <c r="E230" s="7"/>
-      <c r="F230" s="7"/>
+      <c r="E230" s="31"/>
+      <c r="F230" s="31"/>
       <c r="G230" s="31"/>
       <c r="H230" s="31"/>
-      <c r="I230" s="31"/>
+      <c r="I230" s="7"/>
       <c r="J230" s="31"/>
       <c r="K230" s="31"/>
       <c r="L230" s="31"/>
@@ -9014,7 +9034,7 @@
       <c r="C231" s="7"/>
       <c r="D231" s="31"/>
       <c r="E231" s="7"/>
-      <c r="F231" s="31"/>
+      <c r="F231" s="7"/>
       <c r="G231" s="31"/>
       <c r="H231" s="31"/>
       <c r="I231" s="31"/>
@@ -9038,33 +9058,33 @@
       <c r="AA231" s="31"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="A232" s="30"/>
-      <c r="B232" s="30"/>
-      <c r="C232" s="30"/>
-      <c r="D232" s="30"/>
-      <c r="E232" s="30"/>
-      <c r="F232" s="30"/>
-      <c r="G232" s="30"/>
-      <c r="H232" s="30"/>
-      <c r="I232" s="30"/>
-      <c r="J232" s="30"/>
-      <c r="K232" s="30"/>
-      <c r="L232" s="30"/>
-      <c r="M232" s="30"/>
-      <c r="N232" s="30"/>
-      <c r="O232" s="30"/>
-      <c r="P232" s="30"/>
-      <c r="Q232" s="30"/>
-      <c r="R232" s="30"/>
-      <c r="S232" s="30"/>
-      <c r="T232" s="30"/>
-      <c r="U232" s="30"/>
-      <c r="V232" s="30"/>
-      <c r="W232" s="30"/>
-      <c r="X232" s="30"/>
-      <c r="Y232" s="30"/>
-      <c r="Z232" s="30"/>
-      <c r="AA232" s="30"/>
+      <c r="A232" s="7"/>
+      <c r="B232" s="7"/>
+      <c r="C232" s="7"/>
+      <c r="D232" s="31"/>
+      <c r="E232" s="7"/>
+      <c r="F232" s="31"/>
+      <c r="G232" s="31"/>
+      <c r="H232" s="31"/>
+      <c r="I232" s="31"/>
+      <c r="J232" s="31"/>
+      <c r="K232" s="31"/>
+      <c r="L232" s="31"/>
+      <c r="M232" s="31"/>
+      <c r="N232" s="31"/>
+      <c r="O232" s="31"/>
+      <c r="P232" s="31"/>
+      <c r="Q232" s="31"/>
+      <c r="R232" s="31"/>
+      <c r="S232" s="31"/>
+      <c r="T232" s="31"/>
+      <c r="U232" s="31"/>
+      <c r="V232" s="31"/>
+      <c r="W232" s="31"/>
+      <c r="X232" s="31"/>
+      <c r="Y232" s="31"/>
+      <c r="Z232" s="31"/>
+      <c r="AA232" s="31"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
       <c r="A233" s="30"/>
@@ -9096,33 +9116,33 @@
       <c r="AA233" s="30"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="A234" s="32"/>
-      <c r="B234" s="32"/>
-      <c r="C234" s="32"/>
-      <c r="D234" s="32"/>
-      <c r="E234" s="32"/>
-      <c r="F234" s="32"/>
-      <c r="G234" s="32"/>
-      <c r="H234" s="32"/>
-      <c r="I234" s="32"/>
-      <c r="J234" s="32"/>
-      <c r="K234" s="32"/>
-      <c r="L234" s="32"/>
-      <c r="M234" s="32"/>
-      <c r="N234" s="32"/>
-      <c r="O234" s="32"/>
-      <c r="P234" s="32"/>
-      <c r="Q234" s="32"/>
-      <c r="R234" s="32"/>
-      <c r="S234" s="32"/>
-      <c r="T234" s="32"/>
-      <c r="U234" s="32"/>
-      <c r="V234" s="32"/>
-      <c r="W234" s="32"/>
-      <c r="X234" s="32"/>
-      <c r="Y234" s="32"/>
-      <c r="Z234" s="32"/>
-      <c r="AA234" s="32"/>
+      <c r="A234" s="30"/>
+      <c r="B234" s="30"/>
+      <c r="C234" s="30"/>
+      <c r="D234" s="30"/>
+      <c r="E234" s="30"/>
+      <c r="F234" s="30"/>
+      <c r="G234" s="30"/>
+      <c r="H234" s="30"/>
+      <c r="I234" s="30"/>
+      <c r="J234" s="30"/>
+      <c r="K234" s="30"/>
+      <c r="L234" s="30"/>
+      <c r="M234" s="30"/>
+      <c r="N234" s="30"/>
+      <c r="O234" s="30"/>
+      <c r="P234" s="30"/>
+      <c r="Q234" s="30"/>
+      <c r="R234" s="30"/>
+      <c r="S234" s="30"/>
+      <c r="T234" s="30"/>
+      <c r="U234" s="30"/>
+      <c r="V234" s="30"/>
+      <c r="W234" s="30"/>
+      <c r="X234" s="30"/>
+      <c r="Y234" s="30"/>
+      <c r="Z234" s="30"/>
+      <c r="AA234" s="30"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
       <c r="A235" s="32"/>
@@ -10923,7 +10943,33 @@
       <c r="AA296" s="32"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
-      <c r="D297" s="33"/>
+      <c r="A297" s="32"/>
+      <c r="B297" s="32"/>
+      <c r="C297" s="32"/>
+      <c r="D297" s="32"/>
+      <c r="E297" s="32"/>
+      <c r="F297" s="32"/>
+      <c r="G297" s="32"/>
+      <c r="H297" s="32"/>
+      <c r="I297" s="32"/>
+      <c r="J297" s="32"/>
+      <c r="K297" s="32"/>
+      <c r="L297" s="32"/>
+      <c r="M297" s="32"/>
+      <c r="N297" s="32"/>
+      <c r="O297" s="32"/>
+      <c r="P297" s="32"/>
+      <c r="Q297" s="32"/>
+      <c r="R297" s="32"/>
+      <c r="S297" s="32"/>
+      <c r="T297" s="32"/>
+      <c r="U297" s="32"/>
+      <c r="V297" s="32"/>
+      <c r="W297" s="32"/>
+      <c r="X297" s="32"/>
+      <c r="Y297" s="32"/>
+      <c r="Z297" s="32"/>
+      <c r="AA297" s="32"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
       <c r="D298" s="33"/>
@@ -12977,60 +13023,63 @@
     <row r="981" ht="15.75" customHeight="1">
       <c r="D981" s="33"/>
     </row>
+    <row r="982" ht="15.75" customHeight="1">
+      <c r="D982" s="33"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:AA981">
+  <conditionalFormatting sqref="A1:AA982">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="calculate">
       <formula>NOT(ISERROR(SEARCH(("calculate"),(A1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AA981">
+  <conditionalFormatting sqref="A1:AA982">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND($A1="begin group", NOT($B1 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AA981">
+  <conditionalFormatting sqref="A1:AA982">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND($A1="end group", $B1 = "", $C1 = "", $D1 = "", $E1 = "", $F1 = "", $G1 = "", $H1 = "", $I1 = "", $J1 = "", $K1 = "", $M1 = "", $N1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AA981">
+  <conditionalFormatting sqref="A1:AA982">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
     <cfRule type="expression" dxfId="4" priority="5">
-      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1071, "begin group") = COUNTIF($A$1:$A$1071, "end group"))</formula>
+      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1072, "begin group") = COUNTIF($A$1:$A$1072, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
     <cfRule type="expression" dxfId="5" priority="6">
-      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1062, "begin group") = COUNTIF($A$1:$A$1071, "end group")))</formula>
+      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1063, "begin group") = COUNTIF($A$1:$A$1072, "end group")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I981">
+  <conditionalFormatting sqref="I1:I982">
     <cfRule type="expression" dxfId="6" priority="7">
       <formula>AND($I1 = "", $A1 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C981">
+  <conditionalFormatting sqref="C1:C982">
     <cfRule type="expression" dxfId="7" priority="8">
       <formula>AND(AND(NOT($A1 = "end group"), NOT($A1 = "end repeat"), NOT($A1 = "")), $C1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B981">
+  <conditionalFormatting sqref="B1:B982">
     <cfRule type="expression" dxfId="8" priority="9">
       <formula>AND(AND(NOT($A1 = "end group"), NOT($A1 = "end repeat"), NOT($A1 = "")), $B1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A981">
+  <conditionalFormatting sqref="A1:A982">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B981">
+  <conditionalFormatting sqref="B2:B982">
     <cfRule type="expression" dxfId="10" priority="11">
-      <formula>COUNTIF($B$2:$B$1070,B2)&gt;1</formula>
+      <formula>COUNTIF($B$2:$B$1071,B2)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
@@ -13093,23 +13142,23 @@
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H981">
+  <conditionalFormatting sqref="H1:H982">
     <cfRule type="expression" dxfId="7" priority="24">
       <formula>AND(NOT($G1 = ""), $H1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AA981">
+  <conditionalFormatting sqref="A1:AA982">
     <cfRule type="expression" dxfId="11" priority="25">
       <formula>AND($A1="begin repeat", NOT($B1 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AA981">
+  <conditionalFormatting sqref="A1:AA982">
     <cfRule type="expression" dxfId="12" priority="26">
       <formula>AND($A1="end repeat", $B1 = "", $C1 = "", $D1 = "", $E1 = "", $F1 = "", $G1 = "", $H1 = "", $I1 = "", $J1 = "", $K1 = "", $M1 = "", $N1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D981">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D982">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13141,7 +13190,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="34" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B1" s="34" t="s">
         <v>1</v>
@@ -13153,80 +13202,80 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="36" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B2" s="36" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="36" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1"/>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="37" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="37" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="37" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="37" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="37" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -13239,10 +13288,10 @@
         <v>96</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -13250,10 +13299,10 @@
         <v>96</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -13261,10 +13310,10 @@
         <v>96</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
@@ -13272,10 +13321,10 @@
         <v>96</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1"/>
@@ -13284,10 +13333,10 @@
         <v>125</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
@@ -13295,10 +13344,10 @@
         <v>125</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -13306,10 +13355,10 @@
         <v>125</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
@@ -13317,10 +13366,10 @@
         <v>125</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
@@ -13328,10 +13377,10 @@
         <v>125</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -13339,10 +13388,10 @@
         <v>125</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -13353,10 +13402,10 @@
         <v>168</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -13364,10 +13413,10 @@
         <v>168</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -13375,10 +13424,10 @@
         <v>168</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -13386,10 +13435,10 @@
         <v>168</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C26" s="39" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -13397,10 +13446,10 @@
         <v>168</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -13408,10 +13457,10 @@
         <v>168</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -13419,10 +13468,10 @@
         <v>168</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1"/>
@@ -14379,40 +14428,40 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="34" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="42" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C2" s="43">
         <f>NOW()</f>
-        <v>44572.3991</v>
+        <v>44599.22144</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F2" s="44"/>
     </row>

</xml_diff>